<commit_message>
added one generic method getPostResponse
</commit_message>
<xml_diff>
--- a/mobile/src/main/resources/Sanity.xlsx
+++ b/mobile/src/main/resources/Sanity.xlsx
@@ -194,10 +194,10 @@
     <t>Verifying Auth Login API</t>
   </si>
   <si>
-    <t>All_APIs</t>
-  </si>
-  <si>
-    <t>3,5-7,14,18,20-22,28-31,34,36,39,41,44,46,47</t>
+    <t>test2_instance</t>
+  </si>
+  <si>
+    <t>1-5,7,9,11-12,14-15,18,20-23,27-40,42,44-48,50,51</t>
   </si>
 </sst>
 </file>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +852,7 @@
       <c r="F14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating latest mobile code
</commit_message>
<xml_diff>
--- a/mobile/src/main/resources/Sanity.xlsx
+++ b/mobile/src/main/resources/Sanity.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>TCID</t>
   </si>
@@ -197,7 +197,10 @@
     <t>wild1_instance</t>
   </si>
   <si>
-    <t>1-10,12-16,20-37,39-43,46-54,56-60,62-63</t>
+    <t>1-10,12-16,20-21,24-31,35-37,39-43,46-54,56-60,62-63</t>
+  </si>
+  <si>
+    <t>1-10,12-14,20-21,24-31,37,39-43,46-54,56-60,62-63</t>
   </si>
 </sst>
 </file>
@@ -853,7 +856,7 @@
         <v>56</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>57</v>

</xml_diff>